<commit_message>
Updates to the standardized flow cytometry data prior to publication to OBIS.
</commit_message>
<xml_diff>
--- a/original_data/2022 IYS Flow Cytometry data by cruise.xlsx
+++ b/original_data/2022 IYS Flow Cytometry data by cruise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlomas\Documents\Research Marine BGC\JPSS\other data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\GitHub\2022-Flow-Cytometry\original_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874C89E1-A563-4B9A-89C5-F4D825ACF475}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670DCF11-CD05-48EE-80DD-77DCE6D4D661}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18672" windowHeight="8208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18672" windowHeight="8208" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tinru" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4586" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4586" uniqueCount="136">
   <si>
     <t>Cruise</t>
   </si>
@@ -433,6 +433,9 @@
   <si>
     <t>Synechococcus biomass (ug C/L)</t>
   </si>
+  <si>
+    <t>593A</t>
+  </si>
 </sst>
 </file>
 
@@ -785,7 +788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U734"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD98"/>
     </sheetView>
   </sheetViews>
@@ -40823,8 +40826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599B604B-ECF1-4894-B3AC-BD0156875C2B}">
   <dimension ref="A3:X601"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -43334,7 +43337,7 @@
         <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="C57" t="s">
         <v>51</v>

</xml_diff>